<commit_message>
updated excel parameter listing
</commit_message>
<xml_diff>
--- a/Excel_documents/parameter_list.xlsx
+++ b/Excel_documents/parameter_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Individual_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Individual_Project\Excel_documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06D2618A-67ED-46F7-8475-5A50F20343E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2C7738-4E90-469A-993D-BDF89FDC03F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{419ABDEB-092B-4F89-B217-9AA2D05EE5DC}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -109,6 +108,24 @@
   </si>
   <si>
     <t>add_new_vehicle_age_threshold</t>
+  </si>
+  <si>
+    <t>max_waiting_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0 - 1000) ticks </t>
+  </si>
+  <si>
+    <t>The maximum amount of time passengers should wait before considering adding a new vehicle</t>
+  </si>
+  <si>
+    <t>maxvehicles</t>
+  </si>
+  <si>
+    <t>The maximum number of buses in a given route</t>
+  </si>
+  <si>
+    <t>(1-10) units</t>
   </si>
 </sst>
 </file>
@@ -502,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36560BB6-1E4C-450B-821C-A4AB0E9FF98C}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -626,6 +643,34 @@
         <v>21</v>
       </c>
     </row>
+    <row r="9" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="21" spans="11:11" x14ac:dyDescent="0.35">
       <c r="K21" s="1"/>
     </row>

</xml_diff>